<commit_message>
Next to show CT in neighbors
</commit_message>
<xml_diff>
--- a/data/Variable_Definitions.xlsx
+++ b/data/Variable_Definitions.xlsx
@@ -603,6 +603,9 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
@@ -611,6 +614,9 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,6 +625,9 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
@@ -627,6 +636,9 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
       <c r="D5" s="1" t="s">
         <v>7</v>
       </c>
@@ -638,6 +650,9 @@
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
@@ -677,6 +692,9 @@
       <c r="B9" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
@@ -688,6 +706,9 @@
       <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
@@ -699,6 +720,9 @@
       <c r="B11" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
@@ -710,6 +734,9 @@
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
@@ -721,6 +748,9 @@
       <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
@@ -732,6 +762,9 @@
       <c r="B14" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>25</v>
       </c>
@@ -743,6 +776,9 @@
       <c r="B15" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>27</v>
       </c>
@@ -754,6 +790,9 @@
       <c r="B16" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
@@ -765,6 +804,9 @@
       <c r="B17" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>31</v>
       </c>
@@ -776,6 +818,9 @@
       <c r="B18" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>33</v>
       </c>
@@ -787,6 +832,9 @@
       <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
       <c r="D19" s="1" t="s">
         <v>35</v>
       </c>
@@ -794,6 +842,9 @@
     <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>37</v>

</xml_diff>